<commit_message>
Enhance player input validation, improve game instructions, and expand location details
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10402"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hoang/Desktop/Programming/COSC2511-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46ADD90C-DF6D-6148-9AED-B33359C215A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D98858-2767-47A0-B8D5-E00815E77689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Bug ID</t>
   </si>
@@ -69,6 +69,33 @@
   </si>
   <si>
     <t>Fixed</t>
+  </si>
+  <si>
+    <t>Game menu caused infinite loop</t>
+  </si>
+  <si>
+    <t>Loop code for menu was out of place</t>
+  </si>
+  <si>
+    <t>Restructured the loops for the separate game menus</t>
+  </si>
+  <si>
+    <t>Game could still start with name field empty</t>
+  </si>
+  <si>
+    <t>No validation for name input</t>
+  </si>
+  <si>
+    <t>Name input validation to check for empty input</t>
+  </si>
+  <si>
+    <t>Current location would not print when first starting game</t>
+  </si>
+  <si>
+    <t>Currentlocation was a separate method</t>
+  </si>
+  <si>
+    <t>gameInstructions updated</t>
   </si>
 </sst>
 </file>
@@ -440,22 +467,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -475,7 +502,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -492,6 +519,66 @@
         <v>9</v>
       </c>
       <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enhance game instructions display and improve location management with additional attributes
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D98858-2767-47A0-B8D5-E00815E77689}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA95FC6-E1E9-4381-AFFA-D704A58FAB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>Bug ID</t>
   </si>
@@ -96,6 +96,15 @@
   </si>
   <si>
     <t>gameInstructions updated</t>
+  </si>
+  <si>
+    <t>Solve command has no input for empty locations</t>
+  </si>
+  <si>
+    <t>No else statement to handle</t>
+  </si>
+  <si>
+    <t>Else statement to handle empty locations added</t>
   </si>
 </sst>
 </file>
@@ -467,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +591,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance game interactions with random ship movement messages and improve location descriptions with new items
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA95FC6-E1E9-4381-AFFA-D704A58FAB55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60568227-784B-4BAA-97AE-60413311E065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
   <si>
     <t>Bug ID</t>
   </si>
@@ -105,6 +105,18 @@
   </si>
   <si>
     <t>Else statement to handle empty locations added</t>
+  </si>
+  <si>
+    <t>Item.getname unable to invoke</t>
+  </si>
+  <si>
+    <t>return value of location item getter was null</t>
+  </si>
+  <si>
+    <t>added item to location</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
@@ -476,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -611,6 +623,26 @@
         <v>10</v>
       </c>
     </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Enhance game interaction by adding 'use' command for item usage and updating location descriptions
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60568227-784B-4BAA-97AE-60413311E065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A08A8B-44F4-4E63-BF02-D0483B818D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>Bug ID</t>
   </si>
@@ -117,6 +117,15 @@
   </si>
   <si>
     <t>fixed</t>
+  </si>
+  <si>
+    <t>command use after cryo core activation displays non unique message</t>
+  </si>
+  <si>
+    <t>wrong if statement order</t>
+  </si>
+  <si>
+    <t>unique eventtriggered message added first in if statement</t>
   </si>
 </sst>
 </file>
@@ -488,16 +497,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.5703125" customWidth="1"/>
+    <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="5" width="47.85546875" bestFit="1" customWidth="1"/>
@@ -643,6 +652,26 @@
         <v>26</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor random initialization in GameMap and enhance location descriptions with varied messages; update App class for Rift Gate usage.
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A08A8B-44F4-4E63-BF02-D0483B818D56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54C15A8-4EF7-4B65-B2CB-5CD4DAED4BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Bug ID</t>
   </si>
@@ -126,6 +126,15 @@
   </si>
   <si>
     <t>unique eventtriggered message added first in if statement</t>
+  </si>
+  <si>
+    <t>look command has no message for empty location</t>
+  </si>
+  <si>
+    <t>empty space location has no long description</t>
+  </si>
+  <si>
+    <t>added various long descriptions with random selection</t>
   </si>
 </sst>
 </file>
@@ -497,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,6 +681,26 @@
         <v>26</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor handleSolve method to include GameMap parameter and improve puzzle solving logic
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B54C15A8-4EF7-4B65-B2CB-5CD4DAED4BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952E7FFC-0AC8-49EC-BEFF-CEBB609B5FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
   <si>
     <t>Bug ID</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>added various long descriptions with random selection</t>
+  </si>
+  <si>
+    <t>Monolith/Strix puzzles can be spammed</t>
+  </si>
+  <si>
+    <t>no event triggering for puzzles</t>
+  </si>
+  <si>
+    <t>After a correct answer, trigger event and reformat checking</t>
   </si>
 </sst>
 </file>
@@ -506,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +527,7 @@
     <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -701,7 +710,28 @@
         <v>26</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor quit confirmation logic for improved user experience and add combat handling in the App class
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{952E7FFC-0AC8-49EC-BEFF-CEBB609B5FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8880E47A-CB22-4F73-85BB-BF15CBFD238A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Bug ID</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>After a correct answer, trigger event and reformat checking</t>
+  </si>
+  <si>
+    <t>quit command accepts characters other than y or n</t>
+  </si>
+  <si>
+    <t>confirmation doesn't enforce y or n</t>
+  </si>
+  <si>
+    <t>Wrap the confirmation in a loop that continues prompting until y or n</t>
   </si>
 </sst>
 </file>
@@ -515,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -527,7 +536,7 @@
     <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
-    <col min="5" max="5" width="53.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="62.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -730,6 +739,26 @@
         <v>26</v>
       </c>
     </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor Location class to include hostility parameter and update GameMap locations accordingly
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8880E47A-CB22-4F73-85BB-BF15CBFD238A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F519F-71AC-4BCD-80DE-0765B600E489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Bug ID</t>
   </si>
@@ -153,6 +153,15 @@
   </si>
   <si>
     <t>Wrap the confirmation in a loop that continues prompting until y or n</t>
+  </si>
+  <si>
+    <t>currentLocation method not printing hostility after location constructor refactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactor Location class to include hostility parameter </t>
+  </si>
+  <si>
+    <t>locationclass wasn’t set up properly</t>
   </si>
 </sst>
 </file>
@@ -524,16 +533,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
     <col min="5" max="5" width="62.85546875" bestFit="1" customWidth="1"/>
@@ -759,6 +768,26 @@
         <v>26</v>
       </c>
     </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Implement combat system and enhance player interactions with enemies
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F519F-71AC-4BCD-80DE-0765B600E489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0215A79-CBEF-4CC9-908D-1889DD39A9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Bug ID</t>
   </si>
@@ -162,6 +162,30 @@
   </si>
   <si>
     <t>locationclass wasn’t set up properly</t>
+  </si>
+  <si>
+    <t>mastermind combat triggered even after correct puzzle</t>
+  </si>
+  <si>
+    <t>puzzle logic removed from combat logic</t>
+  </si>
+  <si>
+    <t>incorrect puzzle logic in combat logic</t>
+  </si>
+  <si>
+    <t>combat infinite loop</t>
+  </si>
+  <si>
+    <t>combat loop incorrectly structured</t>
+  </si>
+  <si>
+    <t>refactored combat loop</t>
+  </si>
+  <si>
+    <t>can still trade with enemies after defeating</t>
+  </si>
+  <si>
+    <t>no enemy death check for trade logic</t>
   </si>
 </sst>
 </file>
@@ -533,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -788,6 +812,60 @@
         <v>26</v>
       </c>
     </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" t="s">
+        <v>43</v>
+      </c>
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Enhance combat system and player interactions: - Update App class to improve game flow and add healing command. - Refactor CombatSystem to include healing functionality and adjust enemy attributes. - Add methods for managing player coordinates and checking item possession. - Improve item descriptions and enemy encounter logic.
</commit_message>
<xml_diff>
--- a/bug report.xlsx
+++ b/bug report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Other computers\My MacBook Pro\Programming\COSC2511-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0215A79-CBEF-4CC9-908D-1889DD39A9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E442FF6-71E5-4E58-AF1B-E17088E2B32E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{927C9744-080E-44CA-B534-FC36411C827F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>Bug ID</t>
   </si>
@@ -186,6 +186,18 @@
   </si>
   <si>
     <t>no enemy death check for trade logic</t>
+  </si>
+  <si>
+    <t>player can still get cryo core even after solving mastermind puzzle</t>
+  </si>
+  <si>
+    <t>combat logic doesn’t check for cryocore in inventory</t>
+  </si>
+  <si>
+    <t>added enemy death check to fight command</t>
+  </si>
+  <si>
+    <t>added cryocore check in combatsystem</t>
   </si>
 </sst>
 </file>
@@ -557,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7865D620-C3D0-4862-8A9B-DE7533B4C5E9}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,7 +580,7 @@
     <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="72.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="62.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -865,6 +877,32 @@
       <c r="D15" t="s">
         <v>49</v>
       </c>
+      <c r="E15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>